<commit_message>
xls2xml - completed series.json
</commit_message>
<xml_diff>
--- a/xls2xml/tests_box/input_box_test_shows.xlsx
+++ b/xls2xml/tests_box/input_box_test_shows.xlsx
@@ -436,7 +436,7 @@
     <t xml:space="preserve">synopsis</t>
   </si>
   <si>
-    <t xml:space="preserve">id_season</t>
+    <t xml:space="preserve">id season</t>
   </si>
   <si>
     <t xml:space="preserve">season</t>
@@ -451,19 +451,19 @@
     <t xml:space="preserve">por:A Lista|eng:The List</t>
   </si>
   <si>
+    <t xml:space="preserve">por:A melhor série de contagem regressiva de esportes. Com temas icônicos focados nos momentos e indivíduos mais memoráveis do esporte.|eng:English Synopsis</t>
+  </si>
+  <si>
     <t xml:space="preserve">3ee50673-3b99-4cf9-8fb2-1ad5223f4688</t>
   </si>
   <si>
-    <t xml:space="preserve">Primeira temporada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82ff8ec9-8466-4d45-bffb-ce1faaf7539b</t>
+    <t xml:space="preserve">por:Primeira temporada|eng:First season</t>
   </si>
   <si>
     <t xml:space="preserve">19e1327c-7c0f-491f-9ef0-0365641cb9a1</t>
   </si>
   <si>
-    <t xml:space="preserve">Segunda temporada</t>
+    <t xml:space="preserve">por:Segunda temporada|eng:Second Season</t>
   </si>
 </sst>
 </file>
@@ -1863,7 +1863,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1913,27 +1913,27 @@
         <v>136</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>59</v>
+        <v>137</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E2" s="8" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>136</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>59</v>
+        <v>137</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>140</v>

</xml_diff>